<commit_message>
added letters box to home
</commit_message>
<xml_diff>
--- a/mf-angular/src/assets/images/metadata/VLLCMetadata.xlsx
+++ b/mf-angular/src/assets/images/metadata/VLLCMetadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="VLLC" sheetId="1" state="visible" r:id="rId2"/>
@@ -205,7 +205,7 @@
     <t xml:space="preserve">177 p. : ill. ; 267 x 217mm</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5</t>
+    <t xml:space="preserve">RF_MS_5C</t>
   </si>
   <si>
     <t xml:space="preserve">RF_MS_5.jpg</t>
@@ -5230,2914 +5230,2914 @@
     <t xml:space="preserve">RF_MS_4_107.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_001.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_002.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_003.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_004.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_005.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_006.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_007.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_008.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_009.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_010.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_011.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_012.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_013.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_014.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_015.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_016.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_017.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_018.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_019.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_020.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_021.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_022.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_023.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_024.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_025.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_026.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_027.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_028.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_029.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_030.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_031.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_032.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_033.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_034.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_035.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_036.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_037</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_037.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_038</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_038.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_039.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_040.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_041.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_042.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_043.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_044.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_045.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_046</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_046.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_047</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_047.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_048</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_048.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_049.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_050.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_051.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_052</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_052.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_053</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_053.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_054</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_054.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_055</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_055.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_056.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_057.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_058</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_058.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_059.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_060.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_061.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_062.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_063.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_064</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_064.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_065.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_066</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_066.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_067.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_068</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_068.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_069.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_070.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_071.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_072.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_073</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_073.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_074.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_075.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_076</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_076.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_077</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_077.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_078</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_078.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_079</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_079.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_080.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_081.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_082.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_083.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_084</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_084.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_085</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_085.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_086</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_086.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_087</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_087.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_088</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_088.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_089.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_090</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_090.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_091</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_091.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_092</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_092.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_093</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_093.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_094</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_094.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_095</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_095.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_096</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_096.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_097</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_097.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_098</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_098.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_099.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_100.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_101.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_102.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_103.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_104.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_105.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_106.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_107.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_108</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_108.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_109.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_110.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_111.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_112.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_113</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_113.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_114.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_115.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_116</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_116.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_117</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_117.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_118.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_119</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_119.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_120.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_121</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_121.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_122.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_123.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_124.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_125.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_126</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_126.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_127.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_128.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_129.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_130.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_131</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_131.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_132.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_133</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_133.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_134</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_134.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_135.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_136</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_136.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_137</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_137.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_138.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_139.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_140.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_141.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_142</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_142.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_143</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_143.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_144</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_144.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_145</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_145.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_146</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_146.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_147</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_147.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_148</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_148.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_149</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_149.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_150.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_151</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_151.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_152</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_152.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_153</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_153.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_154</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_154.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_155</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_155.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_156</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_156.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_157</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_157.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_158</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_158.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_159</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_159.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_160</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_160.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_161</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_161.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_162</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_162.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_163</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_163.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_164</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_164.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_165</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_165.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_166</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_166.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_167</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_167.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_168</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_168.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_169</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_169.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_170</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_170.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_171</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_171.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_172.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_173</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_173.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_174</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_174.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_001.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_002.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_003.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_004.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_005.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_006.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_007.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_008.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_009.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_010.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_011.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_012.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_013.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_014.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_015.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_016.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_017.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_018.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_019.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_020.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_021.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_022.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_023.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_024.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_025.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_026.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_027.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_028.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_029.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_030.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_031.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_032.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_033.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_034.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_035.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_036.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_037.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_038.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_039.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_040.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_041.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_042.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_043.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_044.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_045.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_046.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_047.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_048.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_049.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_050.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_051.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_052.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_053.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_054.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_055.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_056.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_057.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_058.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_059.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_060.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_061.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_062.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_063.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_064.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_065.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_066.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_067.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_068.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_069.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_070.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_071.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_072.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_073.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_074.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_075.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_076.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_077.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_078.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_079.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_080.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_081.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_082.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_083.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_084.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_085.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_086.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_087.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_088.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_089.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_090.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_091.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_092</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_092.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_093.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_094.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_095.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_096.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_097.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_098.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_099.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_100.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_101.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_102.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_103.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_104.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_105.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_106.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_107.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_108.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_109.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_110.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_111.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_112.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_113.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_114.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_115.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_116.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_117.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_118.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_119.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_120.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_121.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_122.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_123.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_124.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_125.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_126.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_127.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_128.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_129.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_130.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_131.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_132.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_133.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_134.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_135.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_136.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_137.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_138.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_139.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_140.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_141.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_142.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_143.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_144.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_145.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_146.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_147.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_148.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_149.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_150.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_151.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_152.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_153.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_154.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_155.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_156.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_157.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_158.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_159.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_160.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_161.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_162.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_163</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_163.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_164.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_165.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_166.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_167.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_168.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_169.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_170.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_171.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_172.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_173.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_174.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 173</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_175.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_175.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 174</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_176</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_176.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_176.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 175</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_177</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_177.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_177.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 176</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_178</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_178.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_178.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 177</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_179.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_179.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 178</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_180.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_180.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 179</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_181</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_181.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_181.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 180</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_182</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_182.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_182.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 181</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_183.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_183.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 182</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_184</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_184.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_184.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 183</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_185</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_185.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_185.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 184</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_186</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_186.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_186.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 185</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_187</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_187.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_187.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 186</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_188.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_188.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 187</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_189</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_189.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_189.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 188</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_190</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_190.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_190.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 189</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_191</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_191.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_191.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 190</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_192</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_192.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_192.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 191</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_193</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_193.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_193.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 192</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_194</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_194.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_194</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_194.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 193</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_195</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_195.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_195.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 194</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_196</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_196.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_196.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 195</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_197</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_197.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_197</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_197.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 196</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_198</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_198.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_198.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 197</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_199</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_199.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_199.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 198</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_200.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_200.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 199</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_201.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_201.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 200</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_202</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_202.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_202.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 201</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_203.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_203.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 202</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_204</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_204.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_204.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 203</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_205.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_205.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 204</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_206.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_206.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 205</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_207</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_207.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_207.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 206</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_208</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_208.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_208.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 207</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_209.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_209.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 208</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_210.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_210.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 209</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_211</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_211.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_211.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 210</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_212</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_212.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_212.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 211</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_213</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_213.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_213.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 212</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_214</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_214.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_214.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 213</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_215</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_215.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_215.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 214</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_216</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_216.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_216.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 215</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_217</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_217.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_217.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 216</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_218</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_218.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_218.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 217</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_219</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_219.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_219.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 218</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_220.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_220.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 219</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_221</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_221.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_221.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 220</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_222.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_222.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 221</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_223</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_223.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_223.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 222</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_224.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_224.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 223</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_225</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_225.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_225.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 224</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_226</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_226.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_226.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 225</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_227</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_227.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_227.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 226</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_228</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_228.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_228.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 227</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_229</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_229.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_229.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 228</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_230</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_230.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_230.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 229</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_231</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_231.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_231.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 230</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_232</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_232.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_232.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 231</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_233.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_233.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 232</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_234.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_234.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 233</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_235.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_235.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 234</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_236</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_236.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_236.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 235</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_237</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_237.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_237.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 236</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_238</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_238.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_238.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 237</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_239</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_239.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_239.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 238</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_240</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_240.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_240.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 239</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_241</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_241.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_241.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 240</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_242</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_242.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_242.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 241</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_243</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_243.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_243.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 242</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_244</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_244.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_244.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 243</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_245</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_245.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_245.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 244</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_246</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_246.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_246.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 245</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_247</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_247.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_247.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 246</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_248</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_248.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_248.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 247</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_249</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_249.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_249.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 248</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_250.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_250.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 249</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_251</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_251.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_251.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 250</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_252.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_252.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 251</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_253</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_253.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_253.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 252</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_254.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_254.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 253</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_255.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_255.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 254</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_256</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_256.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_256.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 255</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_257</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_257.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_257.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 256</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_258</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_258.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_258.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 257</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_259</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_259.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_259.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 258</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_260</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_260.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_260.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 259</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_261</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_261.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_261.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 260</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_262</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_262.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_262</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_262.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 261</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_263</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_263.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_263.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 262</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_264</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_264.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_264</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_264.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 263</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_265</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_265.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_265.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 264</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_266</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_266.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_266.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 265</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_267</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_267.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_267.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 266</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_268</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_268.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_268.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 267</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_269</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_269.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_269</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_269.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 268</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_270</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_270.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_270.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 269</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_271</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_271.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_271.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 270</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_272</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_272.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_272</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_272.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 271</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_273</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_273.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_273</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_273.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 272</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_274</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_274.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_274</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_274.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 273</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_275</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_275.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_275.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 274</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_276</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_276.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_276.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 275</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_277</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_277.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_277</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_277.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 276</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_278</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_278.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_278</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_278.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 277</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_279</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_279.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_279</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_279.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 278</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_280</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_280.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_280.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 279</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_281</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_281.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_281.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 280</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_282</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_282.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_282</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_282.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 281</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_283</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_283.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_283</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_283.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 282</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_284</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_284.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_284</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_284.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 283</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_285</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_285.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_285.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 284</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_286</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_286.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_286.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 285</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_287</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_287.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_287</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_287.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 286</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_288</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_288.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_288</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_288.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 287</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_289</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_289.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_289</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_289.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 288</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_290</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_290.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_290</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_290.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 289</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_291</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_291.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_291.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 290</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_292</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_292.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_292</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_292.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 291</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_293</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_293.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_293</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_293.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 292</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_294</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_294.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_294</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_294.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 293</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_295</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_295.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_295.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 294</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_296</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_296.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_296.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 295</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_297</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_297.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_297.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 296</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_298</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_298.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_298.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 297</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_299</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_299.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_299</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_299.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 298</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_300.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_300.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 299</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_301</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_301.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_301.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 300</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_302.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_302.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 301</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_303</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_303.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_303.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 302</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_304</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_304.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_304.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 303</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_305</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_305.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_305.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 304</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_306</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_306.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_306.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 305</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_307</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_307.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_307.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 306</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_308.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_308.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 307</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_309</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_309.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_309.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 308</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_310</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_310.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_310.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 309</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_311</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_311.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_311.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 310</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_312</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_312.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_312.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 311</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_313</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_313.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_313</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_313.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 312</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_314</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_314.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_314</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_314.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 313</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_315</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_315.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_315</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_315.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 314</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_316</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_316.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_316</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_316.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 315</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_317</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_317.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_317</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_317.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 316</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_318</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_318.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_318.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 317</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_319</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_319.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_319.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 318</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_320.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_320.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 319</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_321.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_321.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 320</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_322</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_322.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_322.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 321</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_323.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_323.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 322</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_324</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_324.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_324.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 323</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_325</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_325.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_325.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 324</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_326</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_326.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_326.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 325</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_327</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_327.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_327.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 326</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_328</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_328.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_328.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 327</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_329</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_329.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_329</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_329.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 328</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_330</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_330.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_330.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 329</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_331</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_331.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_331.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 330</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_332</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_332.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_332.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 331</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_333</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_333.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_333.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 332</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_334</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_334.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_334</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_334.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 333</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_335.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_335</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_335.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 334</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_336</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_336.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_336</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_336.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 335</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_337.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_337.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 336</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_338</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_338.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_338</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_338.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 337</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_339</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_339.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_339</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_339.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 338</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_340</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_340.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_340.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 339</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_341</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_341.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_341.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 340</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_342</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_342.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_342</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_342.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 341</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_343</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_343.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_343</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_343.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 342</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_344</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_344.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_344.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 343</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_345.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_345.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 344</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_346</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_346.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_346.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 345</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_347</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_347.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_347</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_347.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 346</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_348</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_348.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_348</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_348.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 347</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_349</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_349.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_349.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 348</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_350</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_350.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_350.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 349</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_351</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_351.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_351.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 350</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_352</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_352.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_352</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_352.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 351</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_353</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_353.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_353</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_353.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 352</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_354</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_354.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_354.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 353</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_355</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_355.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_355.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 354</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_356</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_356.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_356.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 355</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_357</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_357.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_357</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_357.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 356</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_358</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_358.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_358.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 357</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_359</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_359.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_359.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 358</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_360.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_360.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 359</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_361</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_361.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_361</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_361.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 360</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_362</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_362.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_362</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_362.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 361</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_363</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_363.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_363</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_363.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 362</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_364</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_364.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_364.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 363</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_365</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_365.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_365.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 364</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_366</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_366.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_366.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 365</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_367</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_367.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_367</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_367.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 366</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_368</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_368.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_368</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_368.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 367</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_369</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_369.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_369</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_369.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 368</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_370</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_370.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_370</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_370.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 369</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_371</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_371.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_371.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 370</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_372</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_372.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_372</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_372.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 371</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_373</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_373.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_373</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_373.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 372</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_374</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_374.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_374</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_374.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 373</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_375</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_375.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_375.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 374</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_376</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_376.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_376</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_376.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 375</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_377</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_377.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_377</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_377.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 376</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_378</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_378.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_378</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_378.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 377</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_379</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_379.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_379</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_379.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Page 378</t>
   </si>
   <si>
-    <t xml:space="preserve">RF_MS_5_380</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_380.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_381</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_381.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_382</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF_MS_5_382.jpg</t>
+    <t xml:space="preserve">RF_MS_5C_380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_380.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_381</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_381.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_382</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF_MS_5C_382.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">RF_MS_6_001</t>
@@ -12167,13 +12167,14 @@
   </sheetPr>
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="1" width="5.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="1" width="5.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="247" min="17" style="1" width="5.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="248" style="0" width="5.1"/>
@@ -20453,8 +20454,8 @@
   </sheetPr>
   <dimension ref="A1:P384"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29209,7 +29210,7 @@
   </sheetPr>
   <dimension ref="A1:P246"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>